<commit_message>
Udpated spreadsheet of test data
</commit_message>
<xml_diff>
--- a/Triangles/Testing/Triangles Worksheet.xlsx
+++ b/Triangles/Testing/Triangles Worksheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swc/Dropbox/UnderGit/cs1440s17-instructor/Homework/HW3/Triangles/Testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swc/Dropbox/UnderGit/cs1440s17-shared/Triangles/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25360" yWindow="4400" windowWidth="21540" windowHeight="17840" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="3900" windowWidth="21540" windowHeight="17840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="51">
   <si>
     <t>x1</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>TRIANGLE #6</t>
+  </si>
+  <si>
+    <t>EDGES</t>
+  </si>
+  <si>
+    <t>-INFINITY</t>
+  </si>
+  <si>
+    <t>INFINITY</t>
   </si>
 </sst>
 </file>
@@ -255,7 +264,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -293,6 +302,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -580,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB63"/>
+  <dimension ref="A1:AB77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="O42" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,7 +611,7 @@
     <col min="18" max="18" width="13.1640625" customWidth="1"/>
     <col min="19" max="19" width="13.33203125" customWidth="1"/>
     <col min="20" max="20" width="13.1640625" customWidth="1"/>
-    <col min="22" max="22" width="16.33203125" customWidth="1"/>
+    <col min="22" max="22" width="10" customWidth="1"/>
     <col min="27" max="27" width="12.33203125" customWidth="1"/>
     <col min="28" max="28" width="12.5" customWidth="1"/>
   </cols>
@@ -772,15 +782,15 @@
         <v>-4</v>
       </c>
       <c r="N4" s="10">
-        <f>J4*J4</f>
+        <f t="shared" ref="N4:P6" si="1">J4*J4</f>
         <v>4</v>
       </c>
       <c r="O4" s="10">
-        <f>K4*K4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P4" s="10">
-        <f>L4*L4</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="R4">
@@ -804,15 +814,15 @@
         <v>2.2360679774997898</v>
       </c>
       <c r="Z4">
-        <f>J4/W4</f>
+        <f t="shared" ref="Z4:AB6" si="2">J4/W4</f>
         <v>0.48507125007266594</v>
       </c>
       <c r="AA4">
-        <f>K4/X4</f>
+        <f t="shared" si="2"/>
         <v>-0.22360679774997896</v>
       </c>
       <c r="AB4">
-        <f>L4/Y4</f>
+        <f t="shared" si="2"/>
         <v>-1.7888543819998317</v>
       </c>
     </row>
@@ -821,15 +831,15 @@
         <v>29</v>
       </c>
       <c r="B5" s="10">
-        <f t="shared" ref="B5:D6" si="1">F4</f>
+        <f t="shared" ref="B5:D6" si="3">F4</f>
         <v>3</v>
       </c>
       <c r="C5" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D5" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="F5" s="10">
@@ -854,15 +864,15 @@
         <v>-1</v>
       </c>
       <c r="N5" s="10">
-        <f>J5*J5</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="O5" s="10">
-        <f>K5*K5</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="P5" s="10">
-        <f>L5*L5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R5">
@@ -886,15 +896,15 @@
         <v>4.2426406871192848</v>
       </c>
       <c r="Z5">
-        <f>J5/W5</f>
+        <f t="shared" si="2"/>
         <v>0.94868329805051377</v>
       </c>
       <c r="AA5">
-        <f>K5/X5</f>
+        <f t="shared" si="2"/>
         <v>0.94868329805051377</v>
       </c>
       <c r="AB5">
-        <f>L5/Y5</f>
+        <f t="shared" si="2"/>
         <v>-0.23570226039551587</v>
       </c>
     </row>
@@ -903,15 +913,15 @@
         <v>30</v>
       </c>
       <c r="B6" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="C6" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="D6" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="F6" s="10">
@@ -939,15 +949,15 @@
         <v>5</v>
       </c>
       <c r="N6" s="10">
-        <f>J6*J6</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="O6" s="10">
-        <f>K6*K6</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="P6" s="10">
-        <f>L6*L6</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="R6">
@@ -971,15 +981,15 @@
         <v>5.3851648071345037</v>
       </c>
       <c r="Z6">
-        <f>J6/W6</f>
+        <f t="shared" si="2"/>
         <v>-0.92847669088525941</v>
       </c>
       <c r="AA6">
-        <f>K6/X6</f>
+        <f t="shared" si="2"/>
         <v>-0.28284271247461901</v>
       </c>
       <c r="AB6">
-        <f>L6/Y6</f>
+        <f t="shared" si="2"/>
         <v>0.92847669088525941</v>
       </c>
     </row>
@@ -1099,27 +1109,27 @@
         <v>0</v>
       </c>
       <c r="J15" s="10">
-        <f t="shared" ref="J15:L17" si="2">F15-B15</f>
+        <f t="shared" ref="J15:L17" si="4">F15-B15</f>
         <v>20</v>
       </c>
       <c r="K15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N15" s="10">
-        <f>J15*J15</f>
+        <f t="shared" ref="N15:P17" si="5">J15*J15</f>
         <v>400</v>
       </c>
       <c r="O15" s="10">
-        <f>K15*K15</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P15" s="10">
-        <f>L15*L15</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R15">
@@ -1143,15 +1153,15 @@
         <v>20</v>
       </c>
       <c r="Z15" t="e">
-        <f>J15/W15</f>
+        <f t="shared" ref="Z15:AB17" si="6">J15/W15</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AA15">
-        <f>K15/X15</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f>L15/Y15</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1160,15 +1170,15 @@
         <v>29</v>
       </c>
       <c r="B16" s="10">
-        <f t="shared" ref="B16:D17" si="3">F15</f>
+        <f t="shared" ref="B16:D17" si="7">F15</f>
         <v>10</v>
       </c>
       <c r="C16" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D16" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F16" s="10">
@@ -1181,27 +1191,27 @@
         <v>0</v>
       </c>
       <c r="J16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-10</v>
       </c>
       <c r="K16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17.32050808</v>
       </c>
       <c r="L16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N16" s="10">
-        <f>J16*J16</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="O16" s="10">
-        <f>K16*K16</f>
+        <f t="shared" si="5"/>
         <v>300.00000014934528</v>
       </c>
       <c r="P16" s="10">
-        <f>L16*L16</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R16">
@@ -1225,15 +1235,15 @@
         <v>20.000000003733632</v>
       </c>
       <c r="Z16">
-        <f>J16/W16</f>
+        <f t="shared" si="6"/>
         <v>-0.57735026904591824</v>
       </c>
       <c r="AA16">
-        <f>K16/X16</f>
+        <f t="shared" si="6"/>
         <v>1.7320508079999999</v>
       </c>
       <c r="AB16">
-        <f>L16/Y16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1242,15 +1252,15 @@
         <v>30</v>
       </c>
       <c r="B17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="C17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>17.32050808</v>
       </c>
       <c r="D17" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F17" s="10">
@@ -1266,27 +1276,27 @@
         <v>0</v>
       </c>
       <c r="J17" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-10</v>
       </c>
       <c r="K17" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-17.32050808</v>
       </c>
       <c r="L17" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N17" s="10">
-        <f>J17*J17</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="O17" s="10">
-        <f>K17*K17</f>
+        <f t="shared" si="5"/>
         <v>300.00000014934528</v>
       </c>
       <c r="P17" s="10">
-        <f>L17*L17</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R17">
@@ -1310,15 +1320,15 @@
         <v>20.000000003733632</v>
       </c>
       <c r="Z17">
-        <f>J17/W17</f>
+        <f t="shared" si="6"/>
         <v>-0.57735026904591824</v>
       </c>
       <c r="AA17">
-        <f>K17/X17</f>
+        <f t="shared" si="6"/>
         <v>-1.7320508079999999</v>
       </c>
       <c r="AB17">
-        <f>L17/Y17</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1439,27 +1449,27 @@
         <v>0</v>
       </c>
       <c r="J25" s="10">
-        <f t="shared" ref="J25:J27" si="4">F25-B25</f>
+        <f t="shared" ref="J25:J27" si="8">F25-B25</f>
         <v>20</v>
       </c>
       <c r="K25" s="10">
-        <f t="shared" ref="K25:K27" si="5">G25-C25</f>
+        <f t="shared" ref="K25:K27" si="9">G25-C25</f>
         <v>0</v>
       </c>
       <c r="L25" s="10">
-        <f t="shared" ref="L25:L27" si="6">H25-D25</f>
+        <f t="shared" ref="L25:L27" si="10">H25-D25</f>
         <v>0</v>
       </c>
       <c r="N25" s="10">
-        <f>J25*J25</f>
+        <f t="shared" ref="N25:P27" si="11">J25*J25</f>
         <v>400</v>
       </c>
       <c r="O25" s="10">
-        <f>K25*K25</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P25" s="10">
-        <f>L25*L25</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R25">
@@ -1483,15 +1493,15 @@
         <v>20</v>
       </c>
       <c r="Z25" t="e">
-        <f>J25/W25</f>
+        <f t="shared" ref="Z25:AB27" si="12">J25/W25</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AA25">
-        <f>K25/X25</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AB25">
-        <f>L25/Y25</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -1500,15 +1510,15 @@
         <v>29</v>
       </c>
       <c r="B26" s="10">
-        <f t="shared" ref="B26:B27" si="7">F25</f>
+        <f t="shared" ref="B26:B27" si="13">F25</f>
         <v>10</v>
       </c>
       <c r="C26" s="10">
-        <f t="shared" ref="C26:C27" si="8">G25</f>
+        <f t="shared" ref="C26:C27" si="14">G25</f>
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <f t="shared" ref="D26:D27" si="9">H25</f>
+        <f t="shared" ref="D26:D27" si="15">H25</f>
         <v>0</v>
       </c>
       <c r="F26" s="10">
@@ -1521,27 +1531,27 @@
         <v>0</v>
       </c>
       <c r="J26" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-10</v>
       </c>
       <c r="K26" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>33</v>
       </c>
       <c r="L26" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N26" s="10">
-        <f>J26*J26</f>
+        <f t="shared" si="11"/>
         <v>100</v>
       </c>
       <c r="O26" s="10">
-        <f>K26*K26</f>
+        <f t="shared" si="11"/>
         <v>1089</v>
       </c>
       <c r="P26" s="10">
-        <f>L26*L26</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R26">
@@ -1565,15 +1575,15 @@
         <v>34.481879299133332</v>
       </c>
       <c r="Z26">
-        <f>J26/W26</f>
+        <f t="shared" si="12"/>
         <v>-0.30303030303030304</v>
       </c>
       <c r="AA26">
-        <f>K26/X26</f>
+        <f t="shared" si="12"/>
         <v>3.3</v>
       </c>
       <c r="AB26">
-        <f>L26/Y26</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -1582,15 +1592,15 @@
         <v>30</v>
       </c>
       <c r="B27" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="C27" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>33</v>
       </c>
       <c r="D27" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F27" s="10">
@@ -1606,27 +1616,27 @@
         <v>0</v>
       </c>
       <c r="J27" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-10</v>
       </c>
       <c r="K27" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-33</v>
       </c>
       <c r="L27" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N27" s="10">
-        <f>J27*J27</f>
+        <f t="shared" si="11"/>
         <v>100</v>
       </c>
       <c r="O27" s="10">
-        <f>K27*K27</f>
+        <f t="shared" si="11"/>
         <v>1089</v>
       </c>
       <c r="P27" s="10">
-        <f>L27*L27</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R27">
@@ -1650,15 +1660,15 @@
         <v>34.481879299133332</v>
       </c>
       <c r="Z27">
-        <f>J27/W27</f>
+        <f t="shared" si="12"/>
         <v>-0.30303030303030304</v>
       </c>
       <c r="AA27">
-        <f>K27/X27</f>
+        <f t="shared" si="12"/>
         <v>-3.3</v>
       </c>
       <c r="AB27">
-        <f>L27/Y27</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -1759,27 +1769,27 @@
         <v>40</v>
       </c>
       <c r="J36" s="10">
-        <f t="shared" ref="J36:J38" si="10">F36-B36</f>
+        <f t="shared" ref="J36:J38" si="16">F36-B36</f>
         <v>9.9499999999999993</v>
       </c>
       <c r="K36" s="10">
-        <f t="shared" ref="K36:K38" si="11">G36-C36</f>
+        <f t="shared" ref="K36:K38" si="17">G36-C36</f>
         <v>-2.85</v>
       </c>
       <c r="L36" s="10">
-        <f t="shared" ref="L36:L38" si="12">H36-D36</f>
+        <f t="shared" ref="L36:L38" si="18">H36-D36</f>
         <v>15</v>
       </c>
       <c r="N36" s="10">
-        <f>J36*J36</f>
+        <f t="shared" ref="N36:P38" si="19">J36*J36</f>
         <v>99.002499999999984</v>
       </c>
       <c r="O36" s="10">
-        <f>K36*K36</f>
+        <f t="shared" si="19"/>
         <v>8.1225000000000005</v>
       </c>
       <c r="P36" s="10">
-        <f>L36*L36</f>
+        <f t="shared" si="19"/>
         <v>225</v>
       </c>
       <c r="R36">
@@ -1796,15 +1806,15 @@
         <v>29</v>
       </c>
       <c r="B37" s="10">
-        <f t="shared" ref="B37:B38" si="13">F36</f>
+        <f t="shared" ref="B37:B38" si="20">F36</f>
         <v>12.25</v>
       </c>
       <c r="C37" s="10">
-        <f t="shared" ref="C37:C38" si="14">G36</f>
+        <f t="shared" ref="C37:C38" si="21">G36</f>
         <v>2.4</v>
       </c>
       <c r="D37" s="10">
-        <f t="shared" ref="D37:D38" si="15">H36</f>
+        <f t="shared" ref="D37:D38" si="22">H36</f>
         <v>40</v>
       </c>
       <c r="F37" s="10">
@@ -1817,27 +1827,27 @@
         <v>3.2</v>
       </c>
       <c r="J37" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-0.25</v>
       </c>
       <c r="K37" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>5.9</v>
       </c>
       <c r="L37" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>-36.799999999999997</v>
       </c>
       <c r="N37" s="10">
-        <f>J37*J37</f>
+        <f t="shared" si="19"/>
         <v>6.25E-2</v>
       </c>
       <c r="O37" s="10">
-        <f>K37*K37</f>
+        <f t="shared" si="19"/>
         <v>34.81</v>
       </c>
       <c r="P37" s="10">
-        <f>L37*L37</f>
+        <f t="shared" si="19"/>
         <v>1354.2399999999998</v>
       </c>
       <c r="R37">
@@ -1854,15 +1864,15 @@
         <v>30</v>
       </c>
       <c r="B38" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>12</v>
       </c>
       <c r="C38" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="D38" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>3.2</v>
       </c>
       <c r="F38" s="10">
@@ -1878,27 +1888,27 @@
         <v>25</v>
       </c>
       <c r="J38" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>-9.6999999999999993</v>
       </c>
       <c r="K38" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>-3.0500000000000007</v>
       </c>
       <c r="L38" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>21.8</v>
       </c>
       <c r="N38" s="10">
-        <f>J38*J38</f>
+        <f t="shared" si="19"/>
         <v>94.089999999999989</v>
       </c>
       <c r="O38" s="10">
-        <f>K38*K38</f>
+        <f t="shared" si="19"/>
         <v>9.3025000000000038</v>
       </c>
       <c r="P38" s="10">
-        <f>L38*L38</f>
+        <f t="shared" si="19"/>
         <v>475.24</v>
       </c>
       <c r="R38">
@@ -2007,27 +2017,27 @@
         <v>5</v>
       </c>
       <c r="J47" s="10">
-        <f t="shared" ref="J47:J49" si="16">F47-B47</f>
+        <f t="shared" ref="J47:J49" si="23">F47-B47</f>
         <v>2</v>
       </c>
       <c r="K47" s="10">
-        <f t="shared" ref="K47:K49" si="17">G47-C47</f>
+        <f t="shared" ref="K47:K49" si="24">G47-C47</f>
         <v>4</v>
       </c>
       <c r="L47" s="10">
-        <f t="shared" ref="L47:L49" si="18">H47-D47</f>
+        <f t="shared" ref="L47:L49" si="25">H47-D47</f>
         <v>5</v>
       </c>
       <c r="N47" s="10">
-        <f>J47*J47</f>
+        <f t="shared" ref="N47:P49" si="26">J47*J47</f>
         <v>4</v>
       </c>
       <c r="O47" s="10">
-        <f>K47*K47</f>
+        <f t="shared" si="26"/>
         <v>16</v>
       </c>
       <c r="P47" s="10">
-        <f>L47*L47</f>
+        <f t="shared" si="26"/>
         <v>25</v>
       </c>
       <c r="R47">
@@ -2044,15 +2054,15 @@
         <v>29</v>
       </c>
       <c r="B48" s="10">
-        <f t="shared" ref="B48:B49" si="19">F47</f>
+        <f t="shared" ref="B48:B49" si="27">F47</f>
         <v>3</v>
       </c>
       <c r="C48" s="10">
-        <f t="shared" ref="C48:C49" si="20">G47</f>
+        <f t="shared" ref="C48:C49" si="28">G47</f>
         <v>4</v>
       </c>
       <c r="D48" s="10">
-        <f t="shared" ref="D48:D49" si="21">H47</f>
+        <f t="shared" ref="D48:D49" si="29">H47</f>
         <v>5</v>
       </c>
       <c r="F48" s="10">
@@ -2065,27 +2075,27 @@
         <v>4</v>
       </c>
       <c r="J48" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>-1</v>
       </c>
       <c r="K48" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-1</v>
       </c>
       <c r="L48" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-1</v>
       </c>
       <c r="N48" s="10">
-        <f>J48*J48</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="O48" s="10">
-        <f>K48*K48</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="P48" s="10">
-        <f>L48*L48</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="R48">
@@ -2102,15 +2112,15 @@
         <v>30</v>
       </c>
       <c r="B49" s="10">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="C49" s="10">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
       <c r="D49" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="29"/>
         <v>4</v>
       </c>
       <c r="F49" s="10">
@@ -2126,27 +2136,27 @@
         <v>0</v>
       </c>
       <c r="J49" s="10">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>-1</v>
       </c>
       <c r="K49" s="10">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-3</v>
       </c>
       <c r="L49" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-4</v>
       </c>
       <c r="N49" s="10">
-        <f>J49*J49</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="O49" s="10">
-        <f>K49*K49</f>
+        <f t="shared" si="26"/>
         <v>9</v>
       </c>
       <c r="P49" s="10">
-        <f>L49*L49</f>
+        <f t="shared" si="26"/>
         <v>16</v>
       </c>
       <c r="R49">
@@ -2255,27 +2265,27 @@
         <v>5</v>
       </c>
       <c r="J58" s="10">
-        <f t="shared" ref="J58:J60" si="22">F58-B58</f>
+        <f t="shared" ref="J58:J60" si="30">F58-B58</f>
         <v>2</v>
       </c>
       <c r="K58" s="10">
-        <f t="shared" ref="K58:K60" si="23">G58-C58</f>
+        <f t="shared" ref="K58:K60" si="31">G58-C58</f>
         <v>-1</v>
       </c>
       <c r="L58" s="10">
-        <f t="shared" ref="L58:L60" si="24">H58-D58</f>
+        <f t="shared" ref="L58:L60" si="32">H58-D58</f>
         <v>5</v>
       </c>
       <c r="N58" s="10">
-        <f>J58*J58</f>
+        <f t="shared" ref="N58:P60" si="33">J58*J58</f>
         <v>4</v>
       </c>
       <c r="O58" s="10">
-        <f>K58*K58</f>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="P58" s="10">
-        <f>L58*L58</f>
+        <f t="shared" si="33"/>
         <v>25</v>
       </c>
       <c r="R58">
@@ -2292,15 +2302,15 @@
         <v>29</v>
       </c>
       <c r="B59" s="10">
-        <f t="shared" ref="B59:B60" si="25">F58</f>
+        <f t="shared" ref="B59:B60" si="34">F58</f>
         <v>3</v>
       </c>
       <c r="C59" s="10">
-        <f t="shared" ref="C59:C60" si="26">G58</f>
+        <f t="shared" ref="C59:C60" si="35">G58</f>
         <v>0</v>
       </c>
       <c r="D59" s="10">
-        <f t="shared" ref="D59:D60" si="27">H58</f>
+        <f t="shared" ref="D59:D60" si="36">H58</f>
         <v>5</v>
       </c>
       <c r="F59" s="10">
@@ -2313,27 +2323,27 @@
         <v>0</v>
       </c>
       <c r="J59" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>-3</v>
       </c>
       <c r="K59" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="L59" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>-5</v>
       </c>
       <c r="N59" s="10">
-        <f>J59*J59</f>
+        <f t="shared" si="33"/>
         <v>9</v>
       </c>
       <c r="O59" s="10">
-        <f>K59*K59</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="P59" s="10">
-        <f>L59*L59</f>
+        <f t="shared" si="33"/>
         <v>25</v>
       </c>
       <c r="R59">
@@ -2350,15 +2360,15 @@
         <v>30</v>
       </c>
       <c r="B60" s="10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="C60" s="10">
-        <f t="shared" si="26"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="D60" s="10">
-        <f t="shared" si="27"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="F60" s="10">
@@ -2374,27 +2384,27 @@
         <v>0</v>
       </c>
       <c r="J60" s="10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="K60" s="10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="L60" s="10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N60" s="10">
-        <f>J60*J60</f>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="O60" s="10">
-        <f>K60*K60</f>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="P60" s="10">
-        <f>L60*L60</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="R60">
@@ -2432,6 +2442,432 @@
         <v>3.8405728739343035</v>
       </c>
     </row>
+    <row r="67" spans="1:24" ht="21" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B68" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K68" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L68" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S68" s="7"/>
+      <c r="T68" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="V68" t="s">
+        <v>15</v>
+      </c>
+      <c r="W68" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="X68" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" s="10">
+        <v>10</v>
+      </c>
+      <c r="C70" s="10">
+        <v>0</v>
+      </c>
+      <c r="D70" s="10">
+        <v>0</v>
+      </c>
+      <c r="F70" s="10">
+        <v>0</v>
+      </c>
+      <c r="G70" s="10">
+        <v>0</v>
+      </c>
+      <c r="H70" s="10">
+        <v>0</v>
+      </c>
+      <c r="J70" s="10">
+        <f t="shared" ref="J70:J71" si="37">F70-B70</f>
+        <v>-10</v>
+      </c>
+      <c r="K70" s="10">
+        <f t="shared" ref="K70:K71" si="38">G70-C70</f>
+        <v>0</v>
+      </c>
+      <c r="L70" s="10">
+        <f t="shared" ref="L70:L71" si="39">H70-D70</f>
+        <v>0</v>
+      </c>
+      <c r="N70" s="10">
+        <f t="shared" ref="N70:N71" si="40">J70*J70</f>
+        <v>100</v>
+      </c>
+      <c r="O70" s="10">
+        <f t="shared" ref="O70:O71" si="41">K70*K70</f>
+        <v>0</v>
+      </c>
+      <c r="P70" s="10">
+        <f t="shared" ref="P70:P71" si="42">L70*L70</f>
+        <v>0</v>
+      </c>
+      <c r="R70">
+        <f>SQRT(N70 + O70 + P70)</f>
+        <v>10</v>
+      </c>
+      <c r="T70">
+        <f>T74-R70</f>
+        <v>-1.5558248717723977</v>
+      </c>
+      <c r="V70" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="W70">
+        <f>K70/SQRT(J70*J70 + L70*L70)</f>
+        <v>0</v>
+      </c>
+      <c r="X70">
+        <f>L70/SQRT(J70*J70 + K70*K70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" s="10">
+        <f t="shared" ref="B71" si="43">F70</f>
+        <v>0</v>
+      </c>
+      <c r="C71" s="10">
+        <f t="shared" ref="C71" si="44">G70</f>
+        <v>0</v>
+      </c>
+      <c r="D71" s="10">
+        <v>1</v>
+      </c>
+      <c r="F71" s="10">
+        <v>10</v>
+      </c>
+      <c r="G71" s="10">
+        <v>0</v>
+      </c>
+      <c r="H71" s="10">
+        <v>1</v>
+      </c>
+      <c r="J71" s="10">
+        <f t="shared" si="37"/>
+        <v>10</v>
+      </c>
+      <c r="K71" s="10">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="L71" s="10">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="N71" s="10">
+        <f t="shared" si="40"/>
+        <v>100</v>
+      </c>
+      <c r="O71" s="10">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="P71" s="10">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <f>SQRT(N71 + O71 + P71)</f>
+        <v>10</v>
+      </c>
+      <c r="T71">
+        <f>T74-R71</f>
+        <v>-1.5558248717723977</v>
+      </c>
+      <c r="V71" t="s">
+        <v>50</v>
+      </c>
+      <c r="W71">
+        <f>K71/SQRT(J71*J71 + L71*L71)</f>
+        <v>0</v>
+      </c>
+      <c r="X71">
+        <f>L71/SQRT(J71*J71 + K71*K71)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" s="10">
+        <v>10</v>
+      </c>
+      <c r="C72" s="10">
+        <v>0</v>
+      </c>
+      <c r="D72" s="10">
+        <v>0</v>
+      </c>
+      <c r="F72" s="10">
+        <v>0</v>
+      </c>
+      <c r="G72" s="10">
+        <v>1</v>
+      </c>
+      <c r="H72" s="10">
+        <v>2</v>
+      </c>
+      <c r="J72" s="10">
+        <f t="shared" ref="J72:J74" si="45">F72-B72</f>
+        <v>-10</v>
+      </c>
+      <c r="K72" s="10">
+        <f t="shared" ref="K72:K74" si="46">G72-C72</f>
+        <v>1</v>
+      </c>
+      <c r="L72" s="10">
+        <f t="shared" ref="L72:L74" si="47">H72-D72</f>
+        <v>2</v>
+      </c>
+      <c r="N72" s="10">
+        <f t="shared" ref="N72:N74" si="48">J72*J72</f>
+        <v>100</v>
+      </c>
+      <c r="O72" s="10">
+        <f t="shared" ref="O72:O74" si="49">K72*K72</f>
+        <v>1</v>
+      </c>
+      <c r="P72" s="10">
+        <f t="shared" ref="P72:P74" si="50">L72*L72</f>
+        <v>4</v>
+      </c>
+      <c r="R72">
+        <f>SQRT(N72 + O72 + P72)</f>
+        <v>10.246950765959598</v>
+      </c>
+      <c r="T72">
+        <f>T76-R72</f>
+        <v>1.8027756377319939</v>
+      </c>
+      <c r="V72">
+        <f>J72/SQRT(K72*K72 + L72*L72)</f>
+        <v>-4.4721359549995796</v>
+      </c>
+      <c r="W72">
+        <f>K72/SQRT(J72*J72 + L72*L72)</f>
+        <v>9.8058067569092022E-2</v>
+      </c>
+      <c r="X72">
+        <f>L72/SQRT(J72*J72 + K72*K72)</f>
+        <v>0.19900743804199783</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>29</v>
+      </c>
+      <c r="B73" s="10">
+        <f t="shared" ref="B73:B74" si="51">F72</f>
+        <v>0</v>
+      </c>
+      <c r="C73" s="10">
+        <f t="shared" ref="C73:C74" si="52">G72</f>
+        <v>1</v>
+      </c>
+      <c r="D73" s="10">
+        <v>1</v>
+      </c>
+      <c r="F73" s="10">
+        <v>10</v>
+      </c>
+      <c r="G73" s="10">
+        <v>2</v>
+      </c>
+      <c r="H73" s="10">
+        <v>3</v>
+      </c>
+      <c r="J73" s="10">
+        <f t="shared" si="45"/>
+        <v>10</v>
+      </c>
+      <c r="K73" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="L73" s="10">
+        <f t="shared" si="47"/>
+        <v>2</v>
+      </c>
+      <c r="N73" s="10">
+        <f t="shared" si="48"/>
+        <v>100</v>
+      </c>
+      <c r="O73" s="10">
+        <f t="shared" si="49"/>
+        <v>1</v>
+      </c>
+      <c r="P73" s="10">
+        <f t="shared" si="50"/>
+        <v>4</v>
+      </c>
+      <c r="R73">
+        <f>SQRT(N73 + O73 + P73)</f>
+        <v>10.246950765959598</v>
+      </c>
+      <c r="T73">
+        <f>T76-R73</f>
+        <v>1.8027756377319939</v>
+      </c>
+      <c r="V73">
+        <f>J73/SQRT(K73*K73 + L73*L73)</f>
+        <v>4.4721359549995796</v>
+      </c>
+      <c r="W73">
+        <f>K73/SQRT(J73*J73 + L73*L73)</f>
+        <v>9.8058067569092022E-2</v>
+      </c>
+      <c r="X73">
+        <f>L73/SQRT(J73*J73 + K73*K73)</f>
+        <v>0.19900743804199783</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" s="10">
+        <f t="shared" si="51"/>
+        <v>10</v>
+      </c>
+      <c r="C74" s="10">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="D74" s="10">
+        <f t="shared" ref="D74" si="53">H73</f>
+        <v>3</v>
+      </c>
+      <c r="F74" s="10">
+        <f>B72</f>
+        <v>10</v>
+      </c>
+      <c r="G74" s="10">
+        <f>C72</f>
+        <v>0</v>
+      </c>
+      <c r="H74" s="10">
+        <f>D72</f>
+        <v>0</v>
+      </c>
+      <c r="J74" s="10">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="K74" s="10">
+        <f t="shared" si="46"/>
+        <v>-2</v>
+      </c>
+      <c r="L74" s="10">
+        <f t="shared" si="47"/>
+        <v>-3</v>
+      </c>
+      <c r="N74" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="O74" s="10">
+        <f t="shared" si="49"/>
+        <v>4</v>
+      </c>
+      <c r="P74" s="10">
+        <f t="shared" si="50"/>
+        <v>9</v>
+      </c>
+      <c r="R74">
+        <f>SQRT(N74 + O74 + P74)</f>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="T74">
+        <f>T76-R74</f>
+        <v>8.4441751282276023</v>
+      </c>
+      <c r="V74">
+        <f>J74/SQRT(K74*K74 + L74*L74)</f>
+        <v>0</v>
+      </c>
+      <c r="W74">
+        <f>K74/SQRT(J74*J74 + L74*L74)</f>
+        <v>-0.66666666666666663</v>
+      </c>
+      <c r="X74">
+        <f>L74/SQRT(J74*J74 + K74*K74)</f>
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="M76" s="14"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="14"/>
+      <c r="P76" s="14"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="S76" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T76">
+        <f>SUM(R72:R74)/2</f>
+        <v>12.049726403691592</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="S77" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T77">
+        <f>SQRT(T76*T72*T73*T74)</f>
+        <v>18.184815093918324</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>